<commit_message>
Se ha actualizado la base ReporteMinsaDepartamento.xlsx hasta el 04/09/2020
</commit_message>
<xml_diff>
--- a/ReporteMinsaDepartamento.xlsx
+++ b/ReporteMinsaDepartamento.xlsx
@@ -101111,6 +101111,2710 @@
         <v>44073</v>
       </c>
     </row>
+    <row r="3991">
+      <c r="A3991" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3991" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3991" t="n">
+        <v>103488</v>
+      </c>
+      <c r="D3991" t="n">
+        <v>181810</v>
+      </c>
+      <c r="E3991" t="n">
+        <v>285298</v>
+      </c>
+      <c r="F3991" t="n">
+        <v>11612</v>
+      </c>
+      <c r="G3991" t="n">
+        <v>1409428</v>
+      </c>
+      <c r="H3991" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3992">
+      <c r="A3992" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3992" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3992" t="n">
+        <v>6977</v>
+      </c>
+      <c r="D3992" t="n">
+        <v>20512</v>
+      </c>
+      <c r="E3992" t="n">
+        <v>27489</v>
+      </c>
+      <c r="F3992" t="n">
+        <v>1576</v>
+      </c>
+      <c r="G3992" t="n">
+        <v>106375</v>
+      </c>
+      <c r="H3992" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3993">
+      <c r="A3993" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3993" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3993" t="n">
+        <v>3266</v>
+      </c>
+      <c r="D3993" t="n">
+        <v>19350</v>
+      </c>
+      <c r="E3993" t="n">
+        <v>22616</v>
+      </c>
+      <c r="F3993" t="n">
+        <v>2052</v>
+      </c>
+      <c r="G3993" t="n">
+        <v>115112</v>
+      </c>
+      <c r="H3993" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3994">
+      <c r="A3994" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3994" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3994" t="n">
+        <v>4357</v>
+      </c>
+      <c r="D3994" t="n">
+        <v>28546</v>
+      </c>
+      <c r="E3994" t="n">
+        <v>32903</v>
+      </c>
+      <c r="F3994" t="n">
+        <v>1159</v>
+      </c>
+      <c r="G3994" t="n">
+        <v>190926</v>
+      </c>
+      <c r="H3994" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3995">
+      <c r="A3995" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3995" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3995" t="n">
+        <v>416</v>
+      </c>
+      <c r="D3995" t="n">
+        <v>8592</v>
+      </c>
+      <c r="E3995" t="n">
+        <v>9008</v>
+      </c>
+      <c r="F3995" t="n">
+        <v>229</v>
+      </c>
+      <c r="G3995" t="n">
+        <v>57364</v>
+      </c>
+      <c r="H3995" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3996">
+      <c r="A3996" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3996" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3996" t="n">
+        <v>5230</v>
+      </c>
+      <c r="D3996" t="n">
+        <v>10005</v>
+      </c>
+      <c r="E3996" t="n">
+        <v>15235</v>
+      </c>
+      <c r="F3996" t="n">
+        <v>326</v>
+      </c>
+      <c r="G3996" t="n">
+        <v>85679</v>
+      </c>
+      <c r="H3996" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3997">
+      <c r="A3997" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3997" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3997" t="n">
+        <v>2377</v>
+      </c>
+      <c r="D3997" t="n">
+        <v>19876</v>
+      </c>
+      <c r="E3997" t="n">
+        <v>22253</v>
+      </c>
+      <c r="F3997" t="n">
+        <v>1589</v>
+      </c>
+      <c r="G3997" t="n">
+        <v>92277</v>
+      </c>
+      <c r="H3997" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3998">
+      <c r="A3998" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3998" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3998" t="n">
+        <v>1017</v>
+      </c>
+      <c r="D3998" t="n">
+        <v>27725</v>
+      </c>
+      <c r="E3998" t="n">
+        <v>28742</v>
+      </c>
+      <c r="F3998" t="n">
+        <v>1825</v>
+      </c>
+      <c r="G3998" t="n">
+        <v>111700</v>
+      </c>
+      <c r="H3998" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="3999">
+      <c r="A3999" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3999" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3999" t="n">
+        <v>993</v>
+      </c>
+      <c r="D3999" t="n">
+        <v>9890</v>
+      </c>
+      <c r="E3999" t="n">
+        <v>10883</v>
+      </c>
+      <c r="F3999" t="n">
+        <v>191</v>
+      </c>
+      <c r="G3999" t="n">
+        <v>53617</v>
+      </c>
+      <c r="H3999" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4000">
+      <c r="A4000" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4000" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4000" t="n">
+        <v>3029</v>
+      </c>
+      <c r="D4000" t="n">
+        <v>17984</v>
+      </c>
+      <c r="E4000" t="n">
+        <v>21013</v>
+      </c>
+      <c r="F4000" t="n">
+        <v>1455</v>
+      </c>
+      <c r="G4000" t="n">
+        <v>103402</v>
+      </c>
+      <c r="H4000" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4001">
+      <c r="A4001" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4001" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4001" t="n">
+        <v>2092</v>
+      </c>
+      <c r="D4001" t="n">
+        <v>12903</v>
+      </c>
+      <c r="E4001" t="n">
+        <v>14995</v>
+      </c>
+      <c r="F4001" t="n">
+        <v>654</v>
+      </c>
+      <c r="G4001" t="n">
+        <v>87760</v>
+      </c>
+      <c r="H4001" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4002">
+      <c r="A4002" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4002" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4002" t="n">
+        <v>3462</v>
+      </c>
+      <c r="D4002" t="n">
+        <v>14997</v>
+      </c>
+      <c r="E4002" t="n">
+        <v>18459</v>
+      </c>
+      <c r="F4002" t="n">
+        <v>1170</v>
+      </c>
+      <c r="G4002" t="n">
+        <v>95687</v>
+      </c>
+      <c r="H4002" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4003">
+      <c r="A4003" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4003" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4003" t="n">
+        <v>2586</v>
+      </c>
+      <c r="D4003" t="n">
+        <v>12603</v>
+      </c>
+      <c r="E4003" t="n">
+        <v>15189</v>
+      </c>
+      <c r="F4003" t="n">
+        <v>388</v>
+      </c>
+      <c r="G4003" t="n">
+        <v>83227</v>
+      </c>
+      <c r="H4003" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4004">
+      <c r="A4004" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4004" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4004" t="n">
+        <v>1264</v>
+      </c>
+      <c r="D4004" t="n">
+        <v>10998</v>
+      </c>
+      <c r="E4004" t="n">
+        <v>12262</v>
+      </c>
+      <c r="F4004" t="n">
+        <v>331</v>
+      </c>
+      <c r="G4004" t="n">
+        <v>62047</v>
+      </c>
+      <c r="H4004" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4005">
+      <c r="A4005" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4005" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4005" t="n">
+        <v>364</v>
+      </c>
+      <c r="D4005" t="n">
+        <v>2478</v>
+      </c>
+      <c r="E4005" t="n">
+        <v>2842</v>
+      </c>
+      <c r="F4005" t="n">
+        <v>65</v>
+      </c>
+      <c r="G4005" t="n">
+        <v>36901</v>
+      </c>
+      <c r="H4005" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4006">
+      <c r="A4006" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4006" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4006" t="n">
+        <v>633</v>
+      </c>
+      <c r="D4006" t="n">
+        <v>8123</v>
+      </c>
+      <c r="E4006" t="n">
+        <v>8756</v>
+      </c>
+      <c r="F4006" t="n">
+        <v>237</v>
+      </c>
+      <c r="G4006" t="n">
+        <v>57561</v>
+      </c>
+      <c r="H4006" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4007">
+      <c r="A4007" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4007" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4007" t="n">
+        <v>1405</v>
+      </c>
+      <c r="D4007" t="n">
+        <v>7234</v>
+      </c>
+      <c r="E4007" t="n">
+        <v>8639</v>
+      </c>
+      <c r="F4007" t="n">
+        <v>147</v>
+      </c>
+      <c r="G4007" t="n">
+        <v>53627</v>
+      </c>
+      <c r="H4007" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4008">
+      <c r="A4008" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4008" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4008" t="n">
+        <v>3150</v>
+      </c>
+      <c r="D4008" t="n">
+        <v>12423</v>
+      </c>
+      <c r="E4008" t="n">
+        <v>15573</v>
+      </c>
+      <c r="F4008" t="n">
+        <v>922</v>
+      </c>
+      <c r="G4008" t="n">
+        <v>49873</v>
+      </c>
+      <c r="H4008" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4009">
+      <c r="A4009" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4009" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4009" t="n">
+        <v>2348</v>
+      </c>
+      <c r="D4009" t="n">
+        <v>11326</v>
+      </c>
+      <c r="E4009" t="n">
+        <v>13674</v>
+      </c>
+      <c r="F4009" t="n">
+        <v>661</v>
+      </c>
+      <c r="G4009" t="n">
+        <v>63886</v>
+      </c>
+      <c r="H4009" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4010">
+      <c r="A4010" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4010" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4010" t="n">
+        <v>2120</v>
+      </c>
+      <c r="D4010" t="n">
+        <v>6088</v>
+      </c>
+      <c r="E4010" t="n">
+        <v>8208</v>
+      </c>
+      <c r="F4010" t="n">
+        <v>260</v>
+      </c>
+      <c r="G4010" t="n">
+        <v>43663</v>
+      </c>
+      <c r="H4010" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4011">
+      <c r="A4011" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4011" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4011" t="n">
+        <v>706</v>
+      </c>
+      <c r="D4011" t="n">
+        <v>4008</v>
+      </c>
+      <c r="E4011" t="n">
+        <v>4714</v>
+      </c>
+      <c r="F4011" t="n">
+        <v>83</v>
+      </c>
+      <c r="G4011" t="n">
+        <v>33789</v>
+      </c>
+      <c r="H4011" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4012">
+      <c r="A4012" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4012" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4012" t="n">
+        <v>259</v>
+      </c>
+      <c r="D4012" t="n">
+        <v>3601</v>
+      </c>
+      <c r="E4012" t="n">
+        <v>3860</v>
+      </c>
+      <c r="F4012" t="n">
+        <v>89</v>
+      </c>
+      <c r="G4012" t="n">
+        <v>31676</v>
+      </c>
+      <c r="H4012" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4013">
+      <c r="A4013" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4013" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4013" t="n">
+        <v>648</v>
+      </c>
+      <c r="D4013" t="n">
+        <v>5087</v>
+      </c>
+      <c r="E4013" t="n">
+        <v>5735</v>
+      </c>
+      <c r="F4013" t="n">
+        <v>277</v>
+      </c>
+      <c r="G4013" t="n">
+        <v>25840</v>
+      </c>
+      <c r="H4013" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4014">
+      <c r="A4014" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4014" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4014" t="n">
+        <v>999</v>
+      </c>
+      <c r="D4014" t="n">
+        <v>12769</v>
+      </c>
+      <c r="E4014" t="n">
+        <v>13768</v>
+      </c>
+      <c r="F4014" t="n">
+        <v>297</v>
+      </c>
+      <c r="G4014" t="n">
+        <v>44494</v>
+      </c>
+      <c r="H4014" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4015">
+      <c r="A4015" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4015" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4015" t="n">
+        <v>884</v>
+      </c>
+      <c r="D4015" t="n">
+        <v>5175</v>
+      </c>
+      <c r="E4015" t="n">
+        <v>6059</v>
+      </c>
+      <c r="F4015" t="n">
+        <v>129</v>
+      </c>
+      <c r="G4015" t="n">
+        <v>29684</v>
+      </c>
+      <c r="H4015" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4016">
+      <c r="A4016" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4016" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4016" t="n">
+        <v>5436</v>
+      </c>
+      <c r="D4016" t="n">
+        <v>18428</v>
+      </c>
+      <c r="E4016" t="n">
+        <v>23864</v>
+      </c>
+      <c r="F4016" t="n">
+        <v>1220</v>
+      </c>
+      <c r="G4016" t="n">
+        <v>90247</v>
+      </c>
+      <c r="H4016" s="1" t="n">
+        <v>44074</v>
+      </c>
+    </row>
+    <row r="4017">
+      <c r="A4017" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4017" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4017" t="n">
+        <v>104341</v>
+      </c>
+      <c r="D4017" t="n">
+        <v>182985</v>
+      </c>
+      <c r="E4017" t="n">
+        <v>287326</v>
+      </c>
+      <c r="F4017" t="n">
+        <v>11681</v>
+      </c>
+      <c r="G4017" t="n">
+        <v>1418056</v>
+      </c>
+      <c r="H4017" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4018">
+      <c r="A4018" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4018" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4018" t="n">
+        <v>6992</v>
+      </c>
+      <c r="D4018" t="n">
+        <v>20656</v>
+      </c>
+      <c r="E4018" t="n">
+        <v>27648</v>
+      </c>
+      <c r="F4018" t="n">
+        <v>1579</v>
+      </c>
+      <c r="G4018" t="n">
+        <v>106832</v>
+      </c>
+      <c r="H4018" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4019">
+      <c r="A4019" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4019" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4019" t="n">
+        <v>3297</v>
+      </c>
+      <c r="D4019" t="n">
+        <v>19488</v>
+      </c>
+      <c r="E4019" t="n">
+        <v>22785</v>
+      </c>
+      <c r="F4019" t="n">
+        <v>2057</v>
+      </c>
+      <c r="G4019" t="n">
+        <v>115738</v>
+      </c>
+      <c r="H4019" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4020">
+      <c r="A4020" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4020" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4020" t="n">
+        <v>4396</v>
+      </c>
+      <c r="D4020" t="n">
+        <v>28744</v>
+      </c>
+      <c r="E4020" t="n">
+        <v>33140</v>
+      </c>
+      <c r="F4020" t="n">
+        <v>1170</v>
+      </c>
+      <c r="G4020" t="n">
+        <v>191601</v>
+      </c>
+      <c r="H4020" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4021">
+      <c r="A4021" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4021" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4021" t="n">
+        <v>416</v>
+      </c>
+      <c r="D4021" t="n">
+        <v>8673</v>
+      </c>
+      <c r="E4021" t="n">
+        <v>9089</v>
+      </c>
+      <c r="F4021" t="n">
+        <v>229</v>
+      </c>
+      <c r="G4021" t="n">
+        <v>57542</v>
+      </c>
+      <c r="H4021" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4022">
+      <c r="A4022" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4022" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4022" t="n">
+        <v>5263</v>
+      </c>
+      <c r="D4022" t="n">
+        <v>10116</v>
+      </c>
+      <c r="E4022" t="n">
+        <v>15379</v>
+      </c>
+      <c r="F4022" t="n">
+        <v>330</v>
+      </c>
+      <c r="G4022" t="n">
+        <v>86038</v>
+      </c>
+      <c r="H4022" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4023">
+      <c r="A4023" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4023" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4023" t="n">
+        <v>2379</v>
+      </c>
+      <c r="D4023" t="n">
+        <v>19952</v>
+      </c>
+      <c r="E4023" t="n">
+        <v>22331</v>
+      </c>
+      <c r="F4023" t="n">
+        <v>1593</v>
+      </c>
+      <c r="G4023" t="n">
+        <v>92515</v>
+      </c>
+      <c r="H4023" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4024">
+      <c r="A4024" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4024" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4024" t="n">
+        <v>1017</v>
+      </c>
+      <c r="D4024" t="n">
+        <v>27943</v>
+      </c>
+      <c r="E4024" t="n">
+        <v>28960</v>
+      </c>
+      <c r="F4024" t="n">
+        <v>1830</v>
+      </c>
+      <c r="G4024" t="n">
+        <v>112246</v>
+      </c>
+      <c r="H4024" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4025">
+      <c r="A4025" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4025" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4025" t="n">
+        <v>993</v>
+      </c>
+      <c r="D4025" t="n">
+        <v>9971</v>
+      </c>
+      <c r="E4025" t="n">
+        <v>10964</v>
+      </c>
+      <c r="F4025" t="n">
+        <v>191</v>
+      </c>
+      <c r="G4025" t="n">
+        <v>53813</v>
+      </c>
+      <c r="H4025" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4026">
+      <c r="A4026" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4026" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4026" t="n">
+        <v>3036</v>
+      </c>
+      <c r="D4026" t="n">
+        <v>18221</v>
+      </c>
+      <c r="E4026" t="n">
+        <v>21257</v>
+      </c>
+      <c r="F4026" t="n">
+        <v>1457</v>
+      </c>
+      <c r="G4026" t="n">
+        <v>104145</v>
+      </c>
+      <c r="H4026" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4027">
+      <c r="A4027" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4027" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4027" t="n">
+        <v>2093</v>
+      </c>
+      <c r="D4027" t="n">
+        <v>13018</v>
+      </c>
+      <c r="E4027" t="n">
+        <v>15111</v>
+      </c>
+      <c r="F4027" t="n">
+        <v>656</v>
+      </c>
+      <c r="G4027" t="n">
+        <v>88149</v>
+      </c>
+      <c r="H4027" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4028">
+      <c r="A4028" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4028" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4028" t="n">
+        <v>3499</v>
+      </c>
+      <c r="D4028" t="n">
+        <v>15106</v>
+      </c>
+      <c r="E4028" t="n">
+        <v>18605</v>
+      </c>
+      <c r="F4028" t="n">
+        <v>1171</v>
+      </c>
+      <c r="G4028" t="n">
+        <v>96183</v>
+      </c>
+      <c r="H4028" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4029">
+      <c r="A4029" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4029" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4029" t="n">
+        <v>2589</v>
+      </c>
+      <c r="D4029" t="n">
+        <v>12781</v>
+      </c>
+      <c r="E4029" t="n">
+        <v>15370</v>
+      </c>
+      <c r="F4029" t="n">
+        <v>388</v>
+      </c>
+      <c r="G4029" t="n">
+        <v>83678</v>
+      </c>
+      <c r="H4029" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4030">
+      <c r="A4030" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4030" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4030" t="n">
+        <v>1280</v>
+      </c>
+      <c r="D4030" t="n">
+        <v>11164</v>
+      </c>
+      <c r="E4030" t="n">
+        <v>12444</v>
+      </c>
+      <c r="F4030" t="n">
+        <v>333</v>
+      </c>
+      <c r="G4030" t="n">
+        <v>62550</v>
+      </c>
+      <c r="H4030" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4031">
+      <c r="A4031" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4031" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4031" t="n">
+        <v>365</v>
+      </c>
+      <c r="D4031" t="n">
+        <v>2508</v>
+      </c>
+      <c r="E4031" t="n">
+        <v>2873</v>
+      </c>
+      <c r="F4031" t="n">
+        <v>65</v>
+      </c>
+      <c r="G4031" t="n">
+        <v>37051</v>
+      </c>
+      <c r="H4031" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4032">
+      <c r="A4032" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4032" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4032" t="n">
+        <v>633</v>
+      </c>
+      <c r="D4032" t="n">
+        <v>8188</v>
+      </c>
+      <c r="E4032" t="n">
+        <v>8821</v>
+      </c>
+      <c r="F4032" t="n">
+        <v>239</v>
+      </c>
+      <c r="G4032" t="n">
+        <v>57726</v>
+      </c>
+      <c r="H4032" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4033">
+      <c r="A4033" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4033" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4033" t="n">
+        <v>1405</v>
+      </c>
+      <c r="D4033" t="n">
+        <v>7336</v>
+      </c>
+      <c r="E4033" t="n">
+        <v>8741</v>
+      </c>
+      <c r="F4033" t="n">
+        <v>148</v>
+      </c>
+      <c r="G4033" t="n">
+        <v>53896</v>
+      </c>
+      <c r="H4033" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4034">
+      <c r="A4034" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4034" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4034" t="n">
+        <v>3150</v>
+      </c>
+      <c r="D4034" t="n">
+        <v>12549</v>
+      </c>
+      <c r="E4034" t="n">
+        <v>15699</v>
+      </c>
+      <c r="F4034" t="n">
+        <v>923</v>
+      </c>
+      <c r="G4034" t="n">
+        <v>50134</v>
+      </c>
+      <c r="H4034" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4035">
+      <c r="A4035" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4035" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4035" t="n">
+        <v>2369</v>
+      </c>
+      <c r="D4035" t="n">
+        <v>11426</v>
+      </c>
+      <c r="E4035" t="n">
+        <v>13795</v>
+      </c>
+      <c r="F4035" t="n">
+        <v>664</v>
+      </c>
+      <c r="G4035" t="n">
+        <v>64146</v>
+      </c>
+      <c r="H4035" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4036">
+      <c r="A4036" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4036" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4036" t="n">
+        <v>2131</v>
+      </c>
+      <c r="D4036" t="n">
+        <v>6206</v>
+      </c>
+      <c r="E4036" t="n">
+        <v>8337</v>
+      </c>
+      <c r="F4036" t="n">
+        <v>261</v>
+      </c>
+      <c r="G4036" t="n">
+        <v>43904</v>
+      </c>
+      <c r="H4036" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4037">
+      <c r="A4037" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4037" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4037" t="n">
+        <v>706</v>
+      </c>
+      <c r="D4037" t="n">
+        <v>4094</v>
+      </c>
+      <c r="E4037" t="n">
+        <v>4800</v>
+      </c>
+      <c r="F4037" t="n">
+        <v>83</v>
+      </c>
+      <c r="G4037" t="n">
+        <v>33989</v>
+      </c>
+      <c r="H4037" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4038">
+      <c r="A4038" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4038" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4038" t="n">
+        <v>259</v>
+      </c>
+      <c r="D4038" t="n">
+        <v>3632</v>
+      </c>
+      <c r="E4038" t="n">
+        <v>3891</v>
+      </c>
+      <c r="F4038" t="n">
+        <v>89</v>
+      </c>
+      <c r="G4038" t="n">
+        <v>31773</v>
+      </c>
+      <c r="H4038" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4039">
+      <c r="A4039" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4039" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4039" t="n">
+        <v>648</v>
+      </c>
+      <c r="D4039" t="n">
+        <v>5123</v>
+      </c>
+      <c r="E4039" t="n">
+        <v>5771</v>
+      </c>
+      <c r="F4039" t="n">
+        <v>278</v>
+      </c>
+      <c r="G4039" t="n">
+        <v>25938</v>
+      </c>
+      <c r="H4039" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4040">
+      <c r="A4040" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4040" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4040" t="n">
+        <v>1001</v>
+      </c>
+      <c r="D4040" t="n">
+        <v>12845</v>
+      </c>
+      <c r="E4040" t="n">
+        <v>13846</v>
+      </c>
+      <c r="F4040" t="n">
+        <v>300</v>
+      </c>
+      <c r="G4040" t="n">
+        <v>44667</v>
+      </c>
+      <c r="H4040" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4041">
+      <c r="A4041" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4041" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4041" t="n">
+        <v>884</v>
+      </c>
+      <c r="D4041" t="n">
+        <v>5229</v>
+      </c>
+      <c r="E4041" t="n">
+        <v>6113</v>
+      </c>
+      <c r="F4041" t="n">
+        <v>129</v>
+      </c>
+      <c r="G4041" t="n">
+        <v>29779</v>
+      </c>
+      <c r="H4041" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4042">
+      <c r="A4042" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4042" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4042" t="n">
+        <v>5438</v>
+      </c>
+      <c r="D4042" t="n">
+        <v>18595</v>
+      </c>
+      <c r="E4042" t="n">
+        <v>24033</v>
+      </c>
+      <c r="F4042" t="n">
+        <v>1224</v>
+      </c>
+      <c r="G4042" t="n">
+        <v>90945</v>
+      </c>
+      <c r="H4042" s="1" t="n">
+        <v>44075</v>
+      </c>
+    </row>
+    <row r="4043">
+      <c r="A4043" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4043" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4043" t="n">
+        <v>105770</v>
+      </c>
+      <c r="D4043" t="n">
+        <v>185979</v>
+      </c>
+      <c r="E4043" t="n">
+        <v>291749</v>
+      </c>
+      <c r="F4043" t="n">
+        <v>11859</v>
+      </c>
+      <c r="G4043" t="n">
+        <v>1438926</v>
+      </c>
+      <c r="H4043" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4044">
+      <c r="A4044" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4044" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4044" t="n">
+        <v>7068</v>
+      </c>
+      <c r="D4044" t="n">
+        <v>20990</v>
+      </c>
+      <c r="E4044" t="n">
+        <v>28058</v>
+      </c>
+      <c r="F4044" t="n">
+        <v>1592</v>
+      </c>
+      <c r="G4044" t="n">
+        <v>108062</v>
+      </c>
+      <c r="H4044" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4045">
+      <c r="A4045" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4045" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4045" t="n">
+        <v>3334</v>
+      </c>
+      <c r="D4045" t="n">
+        <v>19819</v>
+      </c>
+      <c r="E4045" t="n">
+        <v>23153</v>
+      </c>
+      <c r="F4045" t="n">
+        <v>2073</v>
+      </c>
+      <c r="G4045" t="n">
+        <v>117334</v>
+      </c>
+      <c r="H4045" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4046">
+      <c r="A4046" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4046" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4046" t="n">
+        <v>4467</v>
+      </c>
+      <c r="D4046" t="n">
+        <v>29553</v>
+      </c>
+      <c r="E4046" t="n">
+        <v>34020</v>
+      </c>
+      <c r="F4046" t="n">
+        <v>1186</v>
+      </c>
+      <c r="G4046" t="n">
+        <v>196202</v>
+      </c>
+      <c r="H4046" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4047">
+      <c r="A4047" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4047" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4047" t="n">
+        <v>426</v>
+      </c>
+      <c r="D4047" t="n">
+        <v>8925</v>
+      </c>
+      <c r="E4047" t="n">
+        <v>9351</v>
+      </c>
+      <c r="F4047" t="n">
+        <v>233</v>
+      </c>
+      <c r="G4047" t="n">
+        <v>58349</v>
+      </c>
+      <c r="H4047" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4048">
+      <c r="A4048" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4048" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4048" t="n">
+        <v>5397</v>
+      </c>
+      <c r="D4048" t="n">
+        <v>10540</v>
+      </c>
+      <c r="E4048" t="n">
+        <v>15937</v>
+      </c>
+      <c r="F4048" t="n">
+        <v>339</v>
+      </c>
+      <c r="G4048" t="n">
+        <v>88175</v>
+      </c>
+      <c r="H4048" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4049">
+      <c r="A4049" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4049" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4049" t="n">
+        <v>2401</v>
+      </c>
+      <c r="D4049" t="n">
+        <v>20194</v>
+      </c>
+      <c r="E4049" t="n">
+        <v>22595</v>
+      </c>
+      <c r="F4049" t="n">
+        <v>1597</v>
+      </c>
+      <c r="G4049" t="n">
+        <v>93562</v>
+      </c>
+      <c r="H4049" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4050">
+      <c r="A4050" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4050" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4050" t="n">
+        <v>1022</v>
+      </c>
+      <c r="D4050" t="n">
+        <v>28652</v>
+      </c>
+      <c r="E4050" t="n">
+        <v>29674</v>
+      </c>
+      <c r="F4050" t="n">
+        <v>1842</v>
+      </c>
+      <c r="G4050" t="n">
+        <v>114743</v>
+      </c>
+      <c r="H4050" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4051">
+      <c r="A4051" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4051" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4051" t="n">
+        <v>993</v>
+      </c>
+      <c r="D4051" t="n">
+        <v>10216</v>
+      </c>
+      <c r="E4051" t="n">
+        <v>11209</v>
+      </c>
+      <c r="F4051" t="n">
+        <v>192</v>
+      </c>
+      <c r="G4051" t="n">
+        <v>54932</v>
+      </c>
+      <c r="H4051" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4052">
+      <c r="A4052" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4052" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4052" t="n">
+        <v>3084</v>
+      </c>
+      <c r="D4052" t="n">
+        <v>18673</v>
+      </c>
+      <c r="E4052" t="n">
+        <v>21757</v>
+      </c>
+      <c r="F4052" t="n">
+        <v>1470</v>
+      </c>
+      <c r="G4052" t="n">
+        <v>106251</v>
+      </c>
+      <c r="H4052" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4053">
+      <c r="A4053" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4053" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4053" t="n">
+        <v>2099</v>
+      </c>
+      <c r="D4053" t="n">
+        <v>13405</v>
+      </c>
+      <c r="E4053" t="n">
+        <v>15504</v>
+      </c>
+      <c r="F4053" t="n">
+        <v>665</v>
+      </c>
+      <c r="G4053" t="n">
+        <v>89189</v>
+      </c>
+      <c r="H4053" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4054">
+      <c r="A4054" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4054" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4054" t="n">
+        <v>3535</v>
+      </c>
+      <c r="D4054" t="n">
+        <v>15444</v>
+      </c>
+      <c r="E4054" t="n">
+        <v>18979</v>
+      </c>
+      <c r="F4054" t="n">
+        <v>1178</v>
+      </c>
+      <c r="G4054" t="n">
+        <v>97648</v>
+      </c>
+      <c r="H4054" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4055">
+      <c r="A4055" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4055" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4055" t="n">
+        <v>2631</v>
+      </c>
+      <c r="D4055" t="n">
+        <v>13181</v>
+      </c>
+      <c r="E4055" t="n">
+        <v>15812</v>
+      </c>
+      <c r="F4055" t="n">
+        <v>397</v>
+      </c>
+      <c r="G4055" t="n">
+        <v>85428</v>
+      </c>
+      <c r="H4055" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4056">
+      <c r="A4056" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4056" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4056" t="n">
+        <v>1296</v>
+      </c>
+      <c r="D4056" t="n">
+        <v>11488</v>
+      </c>
+      <c r="E4056" t="n">
+        <v>12784</v>
+      </c>
+      <c r="F4056" t="n">
+        <v>339</v>
+      </c>
+      <c r="G4056" t="n">
+        <v>63900</v>
+      </c>
+      <c r="H4056" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4057">
+      <c r="A4057" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4057" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4057" t="n">
+        <v>379</v>
+      </c>
+      <c r="D4057" t="n">
+        <v>2654</v>
+      </c>
+      <c r="E4057" t="n">
+        <v>3033</v>
+      </c>
+      <c r="F4057" t="n">
+        <v>67</v>
+      </c>
+      <c r="G4057" t="n">
+        <v>38040</v>
+      </c>
+      <c r="H4057" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4058">
+      <c r="A4058" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4058" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4058" t="n">
+        <v>638</v>
+      </c>
+      <c r="D4058" t="n">
+        <v>8509</v>
+      </c>
+      <c r="E4058" t="n">
+        <v>9147</v>
+      </c>
+      <c r="F4058" t="n">
+        <v>243</v>
+      </c>
+      <c r="G4058" t="n">
+        <v>58919</v>
+      </c>
+      <c r="H4058" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4059">
+      <c r="A4059" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4059" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4059" t="n">
+        <v>1436</v>
+      </c>
+      <c r="D4059" t="n">
+        <v>7587</v>
+      </c>
+      <c r="E4059" t="n">
+        <v>9023</v>
+      </c>
+      <c r="F4059" t="n">
+        <v>153</v>
+      </c>
+      <c r="G4059" t="n">
+        <v>54869</v>
+      </c>
+      <c r="H4059" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4060">
+      <c r="A4060" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4060" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4060" t="n">
+        <v>3156</v>
+      </c>
+      <c r="D4060" t="n">
+        <v>12899</v>
+      </c>
+      <c r="E4060" t="n">
+        <v>16055</v>
+      </c>
+      <c r="F4060" t="n">
+        <v>923</v>
+      </c>
+      <c r="G4060" t="n">
+        <v>50998</v>
+      </c>
+      <c r="H4060" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4061">
+      <c r="A4061" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4061" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4061" t="n">
+        <v>2413</v>
+      </c>
+      <c r="D4061" t="n">
+        <v>11688</v>
+      </c>
+      <c r="E4061" t="n">
+        <v>14101</v>
+      </c>
+      <c r="F4061" t="n">
+        <v>664</v>
+      </c>
+      <c r="G4061" t="n">
+        <v>64653</v>
+      </c>
+      <c r="H4061" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4062">
+      <c r="A4062" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4062" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4062" t="n">
+        <v>2187</v>
+      </c>
+      <c r="D4062" t="n">
+        <v>6425</v>
+      </c>
+      <c r="E4062" t="n">
+        <v>8612</v>
+      </c>
+      <c r="F4062" t="n">
+        <v>267</v>
+      </c>
+      <c r="G4062" t="n">
+        <v>44656</v>
+      </c>
+      <c r="H4062" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4063">
+      <c r="A4063" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4063" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4063" t="n">
+        <v>713</v>
+      </c>
+      <c r="D4063" t="n">
+        <v>4226</v>
+      </c>
+      <c r="E4063" t="n">
+        <v>4939</v>
+      </c>
+      <c r="F4063" t="n">
+        <v>86</v>
+      </c>
+      <c r="G4063" t="n">
+        <v>34681</v>
+      </c>
+      <c r="H4063" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4064">
+      <c r="A4064" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4064" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4064" t="n">
+        <v>259</v>
+      </c>
+      <c r="D4064" t="n">
+        <v>3719</v>
+      </c>
+      <c r="E4064" t="n">
+        <v>3978</v>
+      </c>
+      <c r="F4064" t="n">
+        <v>89</v>
+      </c>
+      <c r="G4064" t="n">
+        <v>32278</v>
+      </c>
+      <c r="H4064" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4065">
+      <c r="A4065" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4065" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4065" t="n">
+        <v>679</v>
+      </c>
+      <c r="D4065" t="n">
+        <v>5198</v>
+      </c>
+      <c r="E4065" t="n">
+        <v>5877</v>
+      </c>
+      <c r="F4065" t="n">
+        <v>280</v>
+      </c>
+      <c r="G4065" t="n">
+        <v>26331</v>
+      </c>
+      <c r="H4065" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4066">
+      <c r="A4066" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4066" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4066" t="n">
+        <v>1003</v>
+      </c>
+      <c r="D4066" t="n">
+        <v>13091</v>
+      </c>
+      <c r="E4066" t="n">
+        <v>14094</v>
+      </c>
+      <c r="F4066" t="n">
+        <v>301</v>
+      </c>
+      <c r="G4066" t="n">
+        <v>45395</v>
+      </c>
+      <c r="H4066" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4067">
+      <c r="A4067" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4067" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4067" t="n">
+        <v>900</v>
+      </c>
+      <c r="D4067" t="n">
+        <v>5393</v>
+      </c>
+      <c r="E4067" t="n">
+        <v>6293</v>
+      </c>
+      <c r="F4067" t="n">
+        <v>129</v>
+      </c>
+      <c r="G4067" t="n">
+        <v>30316</v>
+      </c>
+      <c r="H4067" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4068">
+      <c r="A4068" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4068" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4068" t="n">
+        <v>5478</v>
+      </c>
+      <c r="D4068" t="n">
+        <v>18933</v>
+      </c>
+      <c r="E4068" t="n">
+        <v>24411</v>
+      </c>
+      <c r="F4068" t="n">
+        <v>1241</v>
+      </c>
+      <c r="G4068" t="n">
+        <v>92689</v>
+      </c>
+      <c r="H4068" s="1" t="n">
+        <v>44077</v>
+      </c>
+    </row>
+    <row r="4069">
+      <c r="A4069" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4069" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4069" t="n">
+        <v>106589</v>
+      </c>
+      <c r="D4069" t="n">
+        <v>187631</v>
+      </c>
+      <c r="E4069" t="n">
+        <v>294220</v>
+      </c>
+      <c r="F4069" t="n">
+        <v>11921</v>
+      </c>
+      <c r="G4069" t="n">
+        <v>1452892</v>
+      </c>
+      <c r="H4069" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4070">
+      <c r="A4070" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4070" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4070" t="n">
+        <v>7084</v>
+      </c>
+      <c r="D4070" t="n">
+        <v>21123</v>
+      </c>
+      <c r="E4070" t="n">
+        <v>28207</v>
+      </c>
+      <c r="F4070" t="n">
+        <v>1596</v>
+      </c>
+      <c r="G4070" t="n">
+        <v>108870</v>
+      </c>
+      <c r="H4070" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4071">
+      <c r="A4071" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4071" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4071" t="n">
+        <v>3347</v>
+      </c>
+      <c r="D4071" t="n">
+        <v>19988</v>
+      </c>
+      <c r="E4071" t="n">
+        <v>23335</v>
+      </c>
+      <c r="F4071" t="n">
+        <v>2082</v>
+      </c>
+      <c r="G4071" t="n">
+        <v>118346</v>
+      </c>
+      <c r="H4071" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4072">
+      <c r="A4072" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4072" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4072" t="n">
+        <v>4486</v>
+      </c>
+      <c r="D4072" t="n">
+        <v>29933</v>
+      </c>
+      <c r="E4072" t="n">
+        <v>34419</v>
+      </c>
+      <c r="F4072" t="n">
+        <v>1193</v>
+      </c>
+      <c r="G4072" t="n">
+        <v>198643</v>
+      </c>
+      <c r="H4072" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4073">
+      <c r="A4073" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4073" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4073" t="n">
+        <v>430</v>
+      </c>
+      <c r="D4073" t="n">
+        <v>9077</v>
+      </c>
+      <c r="E4073" t="n">
+        <v>9507</v>
+      </c>
+      <c r="F4073" t="n">
+        <v>235</v>
+      </c>
+      <c r="G4073" t="n">
+        <v>58882</v>
+      </c>
+      <c r="H4073" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4074">
+      <c r="A4074" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4074" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4074" t="n">
+        <v>5406</v>
+      </c>
+      <c r="D4074" t="n">
+        <v>10740</v>
+      </c>
+      <c r="E4074" t="n">
+        <v>16146</v>
+      </c>
+      <c r="F4074" t="n">
+        <v>341</v>
+      </c>
+      <c r="G4074" t="n">
+        <v>89260</v>
+      </c>
+      <c r="H4074" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4075">
+      <c r="A4075" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4075" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4075" t="n">
+        <v>2411</v>
+      </c>
+      <c r="D4075" t="n">
+        <v>20287</v>
+      </c>
+      <c r="E4075" t="n">
+        <v>22698</v>
+      </c>
+      <c r="F4075" t="n">
+        <v>1602</v>
+      </c>
+      <c r="G4075" t="n">
+        <v>94223</v>
+      </c>
+      <c r="H4075" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4076">
+      <c r="A4076" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4076" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4076" t="n">
+        <v>1023</v>
+      </c>
+      <c r="D4076" t="n">
+        <v>29056</v>
+      </c>
+      <c r="E4076" t="n">
+        <v>30079</v>
+      </c>
+      <c r="F4076" t="n">
+        <v>1845</v>
+      </c>
+      <c r="G4076" t="n">
+        <v>116340</v>
+      </c>
+      <c r="H4076" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4077">
+      <c r="A4077" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4077" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4077" t="n">
+        <v>993</v>
+      </c>
+      <c r="D4077" t="n">
+        <v>10327</v>
+      </c>
+      <c r="E4077" t="n">
+        <v>11320</v>
+      </c>
+      <c r="F4077" t="n">
+        <v>192</v>
+      </c>
+      <c r="G4077" t="n">
+        <v>55491</v>
+      </c>
+      <c r="H4077" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4078">
+      <c r="A4078" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4078" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4078" t="n">
+        <v>3099</v>
+      </c>
+      <c r="D4078" t="n">
+        <v>18907</v>
+      </c>
+      <c r="E4078" t="n">
+        <v>22006</v>
+      </c>
+      <c r="F4078" t="n">
+        <v>1481</v>
+      </c>
+      <c r="G4078" t="n">
+        <v>107302</v>
+      </c>
+      <c r="H4078" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4079">
+      <c r="A4079" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4079" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4079" t="n">
+        <v>2111</v>
+      </c>
+      <c r="D4079" t="n">
+        <v>13581</v>
+      </c>
+      <c r="E4079" t="n">
+        <v>15692</v>
+      </c>
+      <c r="F4079" t="n">
+        <v>671</v>
+      </c>
+      <c r="G4079" t="n">
+        <v>90107</v>
+      </c>
+      <c r="H4079" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4080">
+      <c r="A4080" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4080" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4080" t="n">
+        <v>3550</v>
+      </c>
+      <c r="D4080" t="n">
+        <v>15554</v>
+      </c>
+      <c r="E4080" t="n">
+        <v>19104</v>
+      </c>
+      <c r="F4080" t="n">
+        <v>1183</v>
+      </c>
+      <c r="G4080" t="n">
+        <v>98243</v>
+      </c>
+      <c r="H4080" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4081">
+      <c r="A4081" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4081" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4081" t="n">
+        <v>2638</v>
+      </c>
+      <c r="D4081" t="n">
+        <v>13443</v>
+      </c>
+      <c r="E4081" t="n">
+        <v>16081</v>
+      </c>
+      <c r="F4081" t="n">
+        <v>397</v>
+      </c>
+      <c r="G4081" t="n">
+        <v>86894</v>
+      </c>
+      <c r="H4081" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4082">
+      <c r="A4082" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4082" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4082" t="n">
+        <v>1302</v>
+      </c>
+      <c r="D4082" t="n">
+        <v>11672</v>
+      </c>
+      <c r="E4082" t="n">
+        <v>12974</v>
+      </c>
+      <c r="F4082" t="n">
+        <v>344</v>
+      </c>
+      <c r="G4082" t="n">
+        <v>64789</v>
+      </c>
+      <c r="H4082" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4083">
+      <c r="A4083" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4083" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4083" t="n">
+        <v>393</v>
+      </c>
+      <c r="D4083" t="n">
+        <v>2719</v>
+      </c>
+      <c r="E4083" t="n">
+        <v>3112</v>
+      </c>
+      <c r="F4083" t="n">
+        <v>69</v>
+      </c>
+      <c r="G4083" t="n">
+        <v>38585</v>
+      </c>
+      <c r="H4083" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4084">
+      <c r="A4084" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4084" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4084" t="n">
+        <v>650</v>
+      </c>
+      <c r="D4084" t="n">
+        <v>8724</v>
+      </c>
+      <c r="E4084" t="n">
+        <v>9374</v>
+      </c>
+      <c r="F4084" t="n">
+        <v>246</v>
+      </c>
+      <c r="G4084" t="n">
+        <v>59684</v>
+      </c>
+      <c r="H4084" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4085">
+      <c r="A4085" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4085" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4085" t="n">
+        <v>1445</v>
+      </c>
+      <c r="D4085" t="n">
+        <v>7772</v>
+      </c>
+      <c r="E4085" t="n">
+        <v>9217</v>
+      </c>
+      <c r="F4085" t="n">
+        <v>157</v>
+      </c>
+      <c r="G4085" t="n">
+        <v>55497</v>
+      </c>
+      <c r="H4085" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4086">
+      <c r="A4086" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4086" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4086" t="n">
+        <v>3160</v>
+      </c>
+      <c r="D4086" t="n">
+        <v>13036</v>
+      </c>
+      <c r="E4086" t="n">
+        <v>16196</v>
+      </c>
+      <c r="F4086" t="n">
+        <v>924</v>
+      </c>
+      <c r="G4086" t="n">
+        <v>51364</v>
+      </c>
+      <c r="H4086" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4087">
+      <c r="A4087" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4087" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4087" t="n">
+        <v>2434</v>
+      </c>
+      <c r="D4087" t="n">
+        <v>11829</v>
+      </c>
+      <c r="E4087" t="n">
+        <v>14263</v>
+      </c>
+      <c r="F4087" t="n">
+        <v>665</v>
+      </c>
+      <c r="G4087" t="n">
+        <v>65246</v>
+      </c>
+      <c r="H4087" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4088">
+      <c r="A4088" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4088" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4088" t="n">
+        <v>2197</v>
+      </c>
+      <c r="D4088" t="n">
+        <v>6552</v>
+      </c>
+      <c r="E4088" t="n">
+        <v>8749</v>
+      </c>
+      <c r="F4088" t="n">
+        <v>271</v>
+      </c>
+      <c r="G4088" t="n">
+        <v>45126</v>
+      </c>
+      <c r="H4088" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4089">
+      <c r="A4089" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4089" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4089" t="n">
+        <v>713</v>
+      </c>
+      <c r="D4089" t="n">
+        <v>4303</v>
+      </c>
+      <c r="E4089" t="n">
+        <v>5016</v>
+      </c>
+      <c r="F4089" t="n">
+        <v>87</v>
+      </c>
+      <c r="G4089" t="n">
+        <v>35122</v>
+      </c>
+      <c r="H4089" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4090">
+      <c r="A4090" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4090" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4090" t="n">
+        <v>263</v>
+      </c>
+      <c r="D4090" t="n">
+        <v>3776</v>
+      </c>
+      <c r="E4090" t="n">
+        <v>4039</v>
+      </c>
+      <c r="F4090" t="n">
+        <v>91</v>
+      </c>
+      <c r="G4090" t="n">
+        <v>32539</v>
+      </c>
+      <c r="H4090" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4091">
+      <c r="A4091" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4091" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4091" t="n">
+        <v>680</v>
+      </c>
+      <c r="D4091" t="n">
+        <v>5228</v>
+      </c>
+      <c r="E4091" t="n">
+        <v>5908</v>
+      </c>
+      <c r="F4091" t="n">
+        <v>283</v>
+      </c>
+      <c r="G4091" t="n">
+        <v>26569</v>
+      </c>
+      <c r="H4091" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4092">
+      <c r="A4092" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4092" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4092" t="n">
+        <v>1004</v>
+      </c>
+      <c r="D4092" t="n">
+        <v>13200</v>
+      </c>
+      <c r="E4092" t="n">
+        <v>14204</v>
+      </c>
+      <c r="F4092" t="n">
+        <v>301</v>
+      </c>
+      <c r="G4092" t="n">
+        <v>45700</v>
+      </c>
+      <c r="H4092" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4093">
+      <c r="A4093" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4093" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4093" t="n">
+        <v>900</v>
+      </c>
+      <c r="D4093" t="n">
+        <v>5480</v>
+      </c>
+      <c r="E4093" t="n">
+        <v>6380</v>
+      </c>
+      <c r="F4093" t="n">
+        <v>131</v>
+      </c>
+      <c r="G4093" t="n">
+        <v>30613</v>
+      </c>
+      <c r="H4093" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="4094">
+      <c r="A4094" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4094" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4094" t="n">
+        <v>5483</v>
+      </c>
+      <c r="D4094" t="n">
+        <v>19119</v>
+      </c>
+      <c r="E4094" t="n">
+        <v>24602</v>
+      </c>
+      <c r="F4094" t="n">
+        <v>1246</v>
+      </c>
+      <c r="G4094" t="n">
+        <v>93685</v>
+      </c>
+      <c r="H4094" s="1" t="n">
+        <v>44078</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
reporte actualizado al 06_09
</commit_message>
<xml_diff>
--- a/ReporteMinsaDepartamento.xlsx
+++ b/ReporteMinsaDepartamento.xlsx
@@ -103815,6 +103815,1358 @@
         <v>44078</v>
       </c>
     </row>
+    <row r="4095">
+      <c r="A4095" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4095" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4095" t="n">
+        <v>107563</v>
+      </c>
+      <c r="D4095" t="n">
+        <v>189192</v>
+      </c>
+      <c r="E4095" t="n">
+        <v>296755</v>
+      </c>
+      <c r="F4095" t="n">
+        <v>11989</v>
+      </c>
+      <c r="G4095" t="n">
+        <v>1466082</v>
+      </c>
+      <c r="H4095" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4096">
+      <c r="A4096" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4096" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4096" t="n">
+        <v>7113</v>
+      </c>
+      <c r="D4096" t="n">
+        <v>21293</v>
+      </c>
+      <c r="E4096" t="n">
+        <v>28406</v>
+      </c>
+      <c r="F4096" t="n">
+        <v>1600</v>
+      </c>
+      <c r="G4096" t="n">
+        <v>109819</v>
+      </c>
+      <c r="H4096" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4097">
+      <c r="A4097" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4097" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4097" t="n">
+        <v>3371</v>
+      </c>
+      <c r="D4097" t="n">
+        <v>20150</v>
+      </c>
+      <c r="E4097" t="n">
+        <v>23521</v>
+      </c>
+      <c r="F4097" t="n">
+        <v>2091</v>
+      </c>
+      <c r="G4097" t="n">
+        <v>119408</v>
+      </c>
+      <c r="H4097" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4098">
+      <c r="A4098" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4098" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4098" t="n">
+        <v>4500</v>
+      </c>
+      <c r="D4098" t="n">
+        <v>30285</v>
+      </c>
+      <c r="E4098" t="n">
+        <v>34785</v>
+      </c>
+      <c r="F4098" t="n">
+        <v>1199</v>
+      </c>
+      <c r="G4098" t="n">
+        <v>200867</v>
+      </c>
+      <c r="H4098" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4099">
+      <c r="A4099" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4099" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4099" t="n">
+        <v>430</v>
+      </c>
+      <c r="D4099" t="n">
+        <v>9231</v>
+      </c>
+      <c r="E4099" t="n">
+        <v>9661</v>
+      </c>
+      <c r="F4099" t="n">
+        <v>237</v>
+      </c>
+      <c r="G4099" t="n">
+        <v>59357</v>
+      </c>
+      <c r="H4099" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4100">
+      <c r="A4100" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4100" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4100" t="n">
+        <v>5473</v>
+      </c>
+      <c r="D4100" t="n">
+        <v>10962</v>
+      </c>
+      <c r="E4100" t="n">
+        <v>16435</v>
+      </c>
+      <c r="F4100" t="n">
+        <v>342</v>
+      </c>
+      <c r="G4100" t="n">
+        <v>90499</v>
+      </c>
+      <c r="H4100" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4101">
+      <c r="A4101" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4101" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4101" t="n">
+        <v>2430</v>
+      </c>
+      <c r="D4101" t="n">
+        <v>20433</v>
+      </c>
+      <c r="E4101" t="n">
+        <v>22863</v>
+      </c>
+      <c r="F4101" t="n">
+        <v>1606</v>
+      </c>
+      <c r="G4101" t="n">
+        <v>94828</v>
+      </c>
+      <c r="H4101" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4102">
+      <c r="A4102" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4102" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4102" t="n">
+        <v>1024</v>
+      </c>
+      <c r="D4102" t="n">
+        <v>29398</v>
+      </c>
+      <c r="E4102" t="n">
+        <v>30422</v>
+      </c>
+      <c r="F4102" t="n">
+        <v>1848</v>
+      </c>
+      <c r="G4102" t="n">
+        <v>117611</v>
+      </c>
+      <c r="H4102" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4103">
+      <c r="A4103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4103" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4103" t="n">
+        <v>993</v>
+      </c>
+      <c r="D4103" t="n">
+        <v>10485</v>
+      </c>
+      <c r="E4103" t="n">
+        <v>11478</v>
+      </c>
+      <c r="F4103" t="n">
+        <v>192</v>
+      </c>
+      <c r="G4103" t="n">
+        <v>56441</v>
+      </c>
+      <c r="H4103" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4104">
+      <c r="A4104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4104" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4104" t="n">
+        <v>3143</v>
+      </c>
+      <c r="D4104" t="n">
+        <v>19200</v>
+      </c>
+      <c r="E4104" t="n">
+        <v>22343</v>
+      </c>
+      <c r="F4104" t="n">
+        <v>1484</v>
+      </c>
+      <c r="G4104" t="n">
+        <v>108999</v>
+      </c>
+      <c r="H4104" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4105">
+      <c r="A4105" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4105" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4105" t="n">
+        <v>2114</v>
+      </c>
+      <c r="D4105" t="n">
+        <v>13773</v>
+      </c>
+      <c r="E4105" t="n">
+        <v>15887</v>
+      </c>
+      <c r="F4105" t="n">
+        <v>678</v>
+      </c>
+      <c r="G4105" t="n">
+        <v>90960</v>
+      </c>
+      <c r="H4105" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4106">
+      <c r="A4106" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4106" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4106" t="n">
+        <v>3574</v>
+      </c>
+      <c r="D4106" t="n">
+        <v>15659</v>
+      </c>
+      <c r="E4106" t="n">
+        <v>19233</v>
+      </c>
+      <c r="F4106" t="n">
+        <v>1189</v>
+      </c>
+      <c r="G4106" t="n">
+        <v>99239</v>
+      </c>
+      <c r="H4106" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4107">
+      <c r="A4107" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4107" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4107" t="n">
+        <v>2675</v>
+      </c>
+      <c r="D4107" t="n">
+        <v>13650</v>
+      </c>
+      <c r="E4107" t="n">
+        <v>16325</v>
+      </c>
+      <c r="F4107" t="n">
+        <v>400</v>
+      </c>
+      <c r="G4107" t="n">
+        <v>88048</v>
+      </c>
+      <c r="H4107" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4108">
+      <c r="A4108" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4108" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4108" t="n">
+        <v>1303</v>
+      </c>
+      <c r="D4108" t="n">
+        <v>11822</v>
+      </c>
+      <c r="E4108" t="n">
+        <v>13125</v>
+      </c>
+      <c r="F4108" t="n">
+        <v>344</v>
+      </c>
+      <c r="G4108" t="n">
+        <v>65688</v>
+      </c>
+      <c r="H4108" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4109">
+      <c r="A4109" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4109" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4109" t="n">
+        <v>394</v>
+      </c>
+      <c r="D4109" t="n">
+        <v>2854</v>
+      </c>
+      <c r="E4109" t="n">
+        <v>3248</v>
+      </c>
+      <c r="F4109" t="n">
+        <v>69</v>
+      </c>
+      <c r="G4109" t="n">
+        <v>39565</v>
+      </c>
+      <c r="H4109" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4110">
+      <c r="A4110" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4110" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4110" t="n">
+        <v>650</v>
+      </c>
+      <c r="D4110" t="n">
+        <v>8918</v>
+      </c>
+      <c r="E4110" t="n">
+        <v>9568</v>
+      </c>
+      <c r="F4110" t="n">
+        <v>250</v>
+      </c>
+      <c r="G4110" t="n">
+        <v>60392</v>
+      </c>
+      <c r="H4110" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4111">
+      <c r="A4111" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4111" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4111" t="n">
+        <v>1451</v>
+      </c>
+      <c r="D4111" t="n">
+        <v>7856</v>
+      </c>
+      <c r="E4111" t="n">
+        <v>9307</v>
+      </c>
+      <c r="F4111" t="n">
+        <v>159</v>
+      </c>
+      <c r="G4111" t="n">
+        <v>55907</v>
+      </c>
+      <c r="H4111" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4112">
+      <c r="A4112" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4112" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4112" t="n">
+        <v>3160</v>
+      </c>
+      <c r="D4112" t="n">
+        <v>13149</v>
+      </c>
+      <c r="E4112" t="n">
+        <v>16309</v>
+      </c>
+      <c r="F4112" t="n">
+        <v>927</v>
+      </c>
+      <c r="G4112" t="n">
+        <v>51673</v>
+      </c>
+      <c r="H4112" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4113">
+      <c r="A4113" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4113" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4113" t="n">
+        <v>2444</v>
+      </c>
+      <c r="D4113" t="n">
+        <v>11940</v>
+      </c>
+      <c r="E4113" t="n">
+        <v>14384</v>
+      </c>
+      <c r="F4113" t="n">
+        <v>665</v>
+      </c>
+      <c r="G4113" t="n">
+        <v>65605</v>
+      </c>
+      <c r="H4113" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4114">
+      <c r="A4114" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4114" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4114" t="n">
+        <v>2227</v>
+      </c>
+      <c r="D4114" t="n">
+        <v>6705</v>
+      </c>
+      <c r="E4114" t="n">
+        <v>8932</v>
+      </c>
+      <c r="F4114" t="n">
+        <v>273</v>
+      </c>
+      <c r="G4114" t="n">
+        <v>45715</v>
+      </c>
+      <c r="H4114" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4115">
+      <c r="A4115" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4115" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4115" t="n">
+        <v>719</v>
+      </c>
+      <c r="D4115" t="n">
+        <v>4447</v>
+      </c>
+      <c r="E4115" t="n">
+        <v>5166</v>
+      </c>
+      <c r="F4115" t="n">
+        <v>88</v>
+      </c>
+      <c r="G4115" t="n">
+        <v>35731</v>
+      </c>
+      <c r="H4115" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4116">
+      <c r="A4116" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4116" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4116" t="n">
+        <v>263</v>
+      </c>
+      <c r="D4116" t="n">
+        <v>3839</v>
+      </c>
+      <c r="E4116" t="n">
+        <v>4102</v>
+      </c>
+      <c r="F4116" t="n">
+        <v>91</v>
+      </c>
+      <c r="G4116" t="n">
+        <v>32889</v>
+      </c>
+      <c r="H4116" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4117">
+      <c r="A4117" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4117" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4117" t="n">
+        <v>680</v>
+      </c>
+      <c r="D4117" t="n">
+        <v>5268</v>
+      </c>
+      <c r="E4117" t="n">
+        <v>5948</v>
+      </c>
+      <c r="F4117" t="n">
+        <v>283</v>
+      </c>
+      <c r="G4117" t="n">
+        <v>26780</v>
+      </c>
+      <c r="H4117" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4118">
+      <c r="A4118" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4118" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4118" t="n">
+        <v>1004</v>
+      </c>
+      <c r="D4118" t="n">
+        <v>13315</v>
+      </c>
+      <c r="E4118" t="n">
+        <v>14319</v>
+      </c>
+      <c r="F4118" t="n">
+        <v>302</v>
+      </c>
+      <c r="G4118" t="n">
+        <v>46065</v>
+      </c>
+      <c r="H4118" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4119">
+      <c r="A4119" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4119" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4119" t="n">
+        <v>900</v>
+      </c>
+      <c r="D4119" t="n">
+        <v>5518</v>
+      </c>
+      <c r="E4119" t="n">
+        <v>6418</v>
+      </c>
+      <c r="F4119" t="n">
+        <v>131</v>
+      </c>
+      <c r="G4119" t="n">
+        <v>30750</v>
+      </c>
+      <c r="H4119" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4120">
+      <c r="A4120" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4120" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4120" t="n">
+        <v>5513</v>
+      </c>
+      <c r="D4120" t="n">
+        <v>19249</v>
+      </c>
+      <c r="E4120" t="n">
+        <v>24762</v>
+      </c>
+      <c r="F4120" t="n">
+        <v>1250</v>
+      </c>
+      <c r="G4120" t="n">
+        <v>94517</v>
+      </c>
+      <c r="H4120" s="1" t="n">
+        <v>44079</v>
+      </c>
+    </row>
+    <row r="4121">
+      <c r="A4121" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4121" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4121" t="n">
+        <v>108292</v>
+      </c>
+      <c r="D4121" t="n">
+        <v>190622</v>
+      </c>
+      <c r="E4121" t="n">
+        <v>298914</v>
+      </c>
+      <c r="F4121" t="n">
+        <v>12054</v>
+      </c>
+      <c r="G4121" t="n">
+        <v>1475932</v>
+      </c>
+      <c r="H4121" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4122">
+      <c r="A4122" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4122" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4122" t="n">
+        <v>7140</v>
+      </c>
+      <c r="D4122" t="n">
+        <v>21467</v>
+      </c>
+      <c r="E4122" t="n">
+        <v>28607</v>
+      </c>
+      <c r="F4122" t="n">
+        <v>1608</v>
+      </c>
+      <c r="G4122" t="n">
+        <v>110458</v>
+      </c>
+      <c r="H4122" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4123">
+      <c r="A4123" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4123" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4123" t="n">
+        <v>3389</v>
+      </c>
+      <c r="D4123" t="n">
+        <v>20345</v>
+      </c>
+      <c r="E4123" t="n">
+        <v>23734</v>
+      </c>
+      <c r="F4123" t="n">
+        <v>2096</v>
+      </c>
+      <c r="G4123" t="n">
+        <v>120049</v>
+      </c>
+      <c r="H4123" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4124">
+      <c r="A4124" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4124" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4124" t="n">
+        <v>4504</v>
+      </c>
+      <c r="D4124" t="n">
+        <v>30649</v>
+      </c>
+      <c r="E4124" t="n">
+        <v>35153</v>
+      </c>
+      <c r="F4124" t="n">
+        <v>1205</v>
+      </c>
+      <c r="G4124" t="n">
+        <v>202341</v>
+      </c>
+      <c r="H4124" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4125">
+      <c r="A4125" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4125" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4125" t="n">
+        <v>430</v>
+      </c>
+      <c r="D4125" t="n">
+        <v>9339</v>
+      </c>
+      <c r="E4125" t="n">
+        <v>9769</v>
+      </c>
+      <c r="F4125" t="n">
+        <v>238</v>
+      </c>
+      <c r="G4125" t="n">
+        <v>59632</v>
+      </c>
+      <c r="H4125" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4126">
+      <c r="A4126" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4126" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4126" t="n">
+        <v>5509</v>
+      </c>
+      <c r="D4126" t="n">
+        <v>11171</v>
+      </c>
+      <c r="E4126" t="n">
+        <v>16680</v>
+      </c>
+      <c r="F4126" t="n">
+        <v>349</v>
+      </c>
+      <c r="G4126" t="n">
+        <v>91400</v>
+      </c>
+      <c r="H4126" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4127">
+      <c r="A4127" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4127" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4127" t="n">
+        <v>2450</v>
+      </c>
+      <c r="D4127" t="n">
+        <v>20578</v>
+      </c>
+      <c r="E4127" t="n">
+        <v>23028</v>
+      </c>
+      <c r="F4127" t="n">
+        <v>1610</v>
+      </c>
+      <c r="G4127" t="n">
+        <v>95361</v>
+      </c>
+      <c r="H4127" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4128">
+      <c r="A4128" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4128" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4128" t="n">
+        <v>1025</v>
+      </c>
+      <c r="D4128" t="n">
+        <v>29647</v>
+      </c>
+      <c r="E4128" t="n">
+        <v>30672</v>
+      </c>
+      <c r="F4128" t="n">
+        <v>1853</v>
+      </c>
+      <c r="G4128" t="n">
+        <v>118451</v>
+      </c>
+      <c r="H4128" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4129">
+      <c r="A4129" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4129" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4129" t="n">
+        <v>993</v>
+      </c>
+      <c r="D4129" t="n">
+        <v>10618</v>
+      </c>
+      <c r="E4129" t="n">
+        <v>11611</v>
+      </c>
+      <c r="F4129" t="n">
+        <v>194</v>
+      </c>
+      <c r="G4129" t="n">
+        <v>57494</v>
+      </c>
+      <c r="H4129" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4130">
+      <c r="A4130" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4130" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4130" t="n">
+        <v>3168</v>
+      </c>
+      <c r="D4130" t="n">
+        <v>19497</v>
+      </c>
+      <c r="E4130" t="n">
+        <v>22665</v>
+      </c>
+      <c r="F4130" t="n">
+        <v>1486</v>
+      </c>
+      <c r="G4130" t="n">
+        <v>110224</v>
+      </c>
+      <c r="H4130" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4131">
+      <c r="A4131" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4131" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4131" t="n">
+        <v>2114</v>
+      </c>
+      <c r="D4131" t="n">
+        <v>13963</v>
+      </c>
+      <c r="E4131" t="n">
+        <v>16077</v>
+      </c>
+      <c r="F4131" t="n">
+        <v>682</v>
+      </c>
+      <c r="G4131" t="n">
+        <v>91820</v>
+      </c>
+      <c r="H4131" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4132">
+      <c r="A4132" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4132" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4132" t="n">
+        <v>3603</v>
+      </c>
+      <c r="D4132" t="n">
+        <v>15791</v>
+      </c>
+      <c r="E4132" t="n">
+        <v>19394</v>
+      </c>
+      <c r="F4132" t="n">
+        <v>1197</v>
+      </c>
+      <c r="G4132" t="n">
+        <v>99905</v>
+      </c>
+      <c r="H4132" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4133">
+      <c r="A4133" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4133" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4133" t="n">
+        <v>2692</v>
+      </c>
+      <c r="D4133" t="n">
+        <v>13783</v>
+      </c>
+      <c r="E4133" t="n">
+        <v>16475</v>
+      </c>
+      <c r="F4133" t="n">
+        <v>403</v>
+      </c>
+      <c r="G4133" t="n">
+        <v>88728</v>
+      </c>
+      <c r="H4133" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4134">
+      <c r="A4134" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4134" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4134" t="n">
+        <v>1303</v>
+      </c>
+      <c r="D4134" t="n">
+        <v>11982</v>
+      </c>
+      <c r="E4134" t="n">
+        <v>13285</v>
+      </c>
+      <c r="F4134" t="n">
+        <v>346</v>
+      </c>
+      <c r="G4134" t="n">
+        <v>66202</v>
+      </c>
+      <c r="H4134" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4135">
+      <c r="A4135" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4135" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4135" t="n">
+        <v>394</v>
+      </c>
+      <c r="D4135" t="n">
+        <v>2960</v>
+      </c>
+      <c r="E4135" t="n">
+        <v>3354</v>
+      </c>
+      <c r="F4135" t="n">
+        <v>69</v>
+      </c>
+      <c r="G4135" t="n">
+        <v>41182</v>
+      </c>
+      <c r="H4135" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4136">
+      <c r="A4136" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4136" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4136" t="n">
+        <v>650</v>
+      </c>
+      <c r="D4136" t="n">
+        <v>9156</v>
+      </c>
+      <c r="E4136" t="n">
+        <v>9806</v>
+      </c>
+      <c r="F4136" t="n">
+        <v>256</v>
+      </c>
+      <c r="G4136" t="n">
+        <v>61115</v>
+      </c>
+      <c r="H4136" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4137">
+      <c r="A4137" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4137" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4137" t="n">
+        <v>1458</v>
+      </c>
+      <c r="D4137" t="n">
+        <v>8061</v>
+      </c>
+      <c r="E4137" t="n">
+        <v>9519</v>
+      </c>
+      <c r="F4137" t="n">
+        <v>163</v>
+      </c>
+      <c r="G4137" t="n">
+        <v>56412</v>
+      </c>
+      <c r="H4137" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4138">
+      <c r="A4138" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4138" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4138" t="n">
+        <v>3169</v>
+      </c>
+      <c r="D4138" t="n">
+        <v>13315</v>
+      </c>
+      <c r="E4138" t="n">
+        <v>16484</v>
+      </c>
+      <c r="F4138" t="n">
+        <v>929</v>
+      </c>
+      <c r="G4138" t="n">
+        <v>52075</v>
+      </c>
+      <c r="H4138" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4139">
+      <c r="A4139" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4139" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4139" t="n">
+        <v>2469</v>
+      </c>
+      <c r="D4139" t="n">
+        <v>12120</v>
+      </c>
+      <c r="E4139" t="n">
+        <v>14589</v>
+      </c>
+      <c r="F4139" t="n">
+        <v>669</v>
+      </c>
+      <c r="G4139" t="n">
+        <v>66085</v>
+      </c>
+      <c r="H4139" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4140">
+      <c r="A4140" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4140" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4140" t="n">
+        <v>2235</v>
+      </c>
+      <c r="D4140" t="n">
+        <v>6837</v>
+      </c>
+      <c r="E4140" t="n">
+        <v>9072</v>
+      </c>
+      <c r="F4140" t="n">
+        <v>276</v>
+      </c>
+      <c r="G4140" t="n">
+        <v>46331</v>
+      </c>
+      <c r="H4140" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4141">
+      <c r="A4141" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4141" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4141" t="n">
+        <v>719</v>
+      </c>
+      <c r="D4141" t="n">
+        <v>4479</v>
+      </c>
+      <c r="E4141" t="n">
+        <v>5198</v>
+      </c>
+      <c r="F4141" t="n">
+        <v>89</v>
+      </c>
+      <c r="G4141" t="n">
+        <v>35916</v>
+      </c>
+      <c r="H4141" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4142">
+      <c r="A4142" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4142" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4142" t="n">
+        <v>270</v>
+      </c>
+      <c r="D4142" t="n">
+        <v>3882</v>
+      </c>
+      <c r="E4142" t="n">
+        <v>4152</v>
+      </c>
+      <c r="F4142" t="n">
+        <v>92</v>
+      </c>
+      <c r="G4142" t="n">
+        <v>33240</v>
+      </c>
+      <c r="H4142" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4143">
+      <c r="A4143" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4143" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4143" t="n">
+        <v>680</v>
+      </c>
+      <c r="D4143" t="n">
+        <v>5300</v>
+      </c>
+      <c r="E4143" t="n">
+        <v>5980</v>
+      </c>
+      <c r="F4143" t="n">
+        <v>283</v>
+      </c>
+      <c r="G4143" t="n">
+        <v>26916</v>
+      </c>
+      <c r="H4143" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4144">
+      <c r="A4144" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4144" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4144" t="n">
+        <v>1004</v>
+      </c>
+      <c r="D4144" t="n">
+        <v>13385</v>
+      </c>
+      <c r="E4144" t="n">
+        <v>14389</v>
+      </c>
+      <c r="F4144" t="n">
+        <v>302</v>
+      </c>
+      <c r="G4144" t="n">
+        <v>46280</v>
+      </c>
+      <c r="H4144" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4145">
+      <c r="A4145" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4145" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4145" t="n">
+        <v>900</v>
+      </c>
+      <c r="D4145" t="n">
+        <v>5592</v>
+      </c>
+      <c r="E4145" t="n">
+        <v>6492</v>
+      </c>
+      <c r="F4145" t="n">
+        <v>131</v>
+      </c>
+      <c r="G4145" t="n">
+        <v>30966</v>
+      </c>
+      <c r="H4145" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
+    <row r="4146">
+      <c r="A4146" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4146" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4146" t="n">
+        <v>5525</v>
+      </c>
+      <c r="D4146" t="n">
+        <v>19353</v>
+      </c>
+      <c r="E4146" t="n">
+        <v>24878</v>
+      </c>
+      <c r="F4146" t="n">
+        <v>1258</v>
+      </c>
+      <c r="G4146" t="n">
+        <v>95065</v>
+      </c>
+      <c r="H4146" s="1" t="n">
+        <v>44080</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>